<commit_message>
WIP: save changes before rebase
</commit_message>
<xml_diff>
--- a/withoutOutofDomain_samePrompt_25_6/test_case/output_11_6/category_classi_result.xlsx
+++ b/withoutOutofDomain_samePrompt_25_6/test_case/output_11_6/category_classi_result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\seniorProject\term2\output_11_6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\update_project\withoutOutofDomain_samePrompt_25_6\test_case\output_11_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0993BA8-C66D-4CB3-80D4-2268F4C91EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8CA0FA-53FC-4295-88C3-3DD532289564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>